<commit_message>
feat: added factory method
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_hustle2live\Design-Patterns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5E6B1E13-84C2-4272-BE40-458064152DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27E41A7-9136-4610-BDDE-9FC0E4D2AA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33120" yWindow="2760" windowWidth="21600" windowHeight="11295" xr2:uid="{5A060E50-CC17-4E2C-BABD-C91FD7036B38}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Builder</t>
   </si>
@@ -83,12 +83,36 @@
     <t>Abstract Factory рекомендуется использовать, когда: Требуется создавать объекты-продукты разных типов и налаживать между ними взаимодействие
 чтобы ни процесс, ни результат построения подсистемы не был зависим от способа создания в ней объектов,</t>
   </si>
+  <si>
+    <t>Factory method</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Назначение паттерна фабричний метод - бить основой всех порождающих паттернов </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Абстрактной_Фабрики, Билдера, Прототипа и Синглтона</t>
+    </r>
+  </si>
+  <si>
+    <t>классовий метод</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +276,16 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -981,7 +1015,7 @@
   <dimension ref="G7:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,10 +1058,16 @@
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+    <row r="11" spans="7:9" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G12" s="2"/>

</xml_diff>